<commit_message>
LLM question answering result analysis
</commit_message>
<xml_diff>
--- a/data/answer/rank.xlsx
+++ b/data/answer/rank.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tj/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mattis\Desktop\VSCode\rag_for_tcfd_reports\data\answer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899DA8B2-0739-4541-A521-36DCC2EB93D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535F227B-2C56-4B74-B78F-DFD1116320D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34200" windowHeight="21380" xr2:uid="{90DEFA0F-3043-42EB-A899-63307E85EE54}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{90DEFA0F-3043-42EB-A899-63307E85EE54}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -872,14 +872,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Aptos Narrow"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -925,7 +925,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -941,7 +941,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1260,67 +1260,67 @@
   <dimension ref="A1:IO81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:E29"/>
+      <selection activeCell="E1" sqref="E1:CQ1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1"/>
-    <col min="5" max="13" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.125" customWidth="1"/>
+    <col min="4" max="4" width="8.625" customWidth="1"/>
+    <col min="5" max="13" width="2.875" bestFit="1" customWidth="1"/>
     <col min="14" max="26" width="3.5" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="4.5" bestFit="1" customWidth="1"/>
     <col min="29" max="56" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="57" max="58" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="58" width="4.625" bestFit="1" customWidth="1"/>
     <col min="59" max="60" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="61" max="62" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="62" width="4.625" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="4.625" bestFit="1" customWidth="1"/>
     <col min="65" max="74" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="75" max="78" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="75" max="78" width="6.125" bestFit="1" customWidth="1"/>
     <col min="79" max="81" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="4.625" bestFit="1" customWidth="1"/>
     <col min="83" max="85" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="6.125" bestFit="1" customWidth="1"/>
     <col min="87" max="95" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="96" max="104" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="105" max="147" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="148" max="149" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="150" max="165" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="166" max="169" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="170" max="176" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="177" max="177" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="178" max="186" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="187" max="189" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="190" max="190" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="191" max="193" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="194" max="195" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="96" max="104" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="105" max="147" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="148" max="149" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="150" max="165" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="166" max="169" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="170" max="176" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="177" max="177" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="178" max="186" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="187" max="189" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="190" max="190" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="191" max="193" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="194" max="195" width="12.625" bestFit="1" customWidth="1"/>
     <col min="196" max="197" width="6.5" bestFit="1" customWidth="1"/>
     <col min="198" max="198" width="17.5" bestFit="1" customWidth="1"/>
     <col min="199" max="207" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="208" max="210" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="211" max="212" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="213" max="217" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="218" max="218" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="219" max="222" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="223" max="225" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="226" max="226" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="227" max="227" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="228" max="228" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="229" max="229" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="230" max="233" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="234" max="238" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="239" max="239" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="240" max="240" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="241" max="241" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="242" max="243" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="208" max="210" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="211" max="212" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="213" max="217" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="218" max="218" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="219" max="222" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="223" max="225" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="226" max="226" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="227" max="227" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="228" max="228" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="229" max="229" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="230" max="233" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="234" max="238" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="239" max="239" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="240" max="240" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="241" max="241" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="242" max="243" width="12.625" bestFit="1" customWidth="1"/>
     <col min="244" max="244" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="245" max="249" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="245" max="249" width="12.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>187</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>0.94131944444444438</v>
       </c>
     </row>
-    <row r="3" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>191</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>0.94027777777777777</v>
       </c>
     </row>
-    <row r="4" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>257</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>0.88518518518518519</v>
       </c>
     </row>
-    <row r="5" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>166</v>
       </c>
@@ -5041,7 +5041,7 @@
         <v>0.87094907407407407</v>
       </c>
     </row>
-    <row r="6" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>173</v>
       </c>
@@ -5784,7 +5784,7 @@
         <v>0.8666666666666667</v>
       </c>
     </row>
-    <row r="7" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>179</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>0.85844907407407411</v>
       </c>
     </row>
-    <row r="8" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>181</v>
       </c>
@@ -7270,7 +7270,7 @@
         <v>0.85555555555555551</v>
       </c>
     </row>
-    <row r="9" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>177</v>
       </c>
@@ -8007,7 +8007,7 @@
         <v>0.80949074074074079</v>
       </c>
     </row>
-    <row r="10" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>171</v>
       </c>
@@ -8750,7 +8750,7 @@
         <v>0.79965277777777777</v>
       </c>
     </row>
-    <row r="11" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>219</v>
       </c>
@@ -9493,7 +9493,7 @@
         <v>0.79918981481481477</v>
       </c>
     </row>
-    <row r="12" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>175</v>
       </c>
@@ -10236,7 +10236,7 @@
         <v>0.78993055555555547</v>
       </c>
     </row>
-    <row r="13" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>245</v>
       </c>
@@ -10979,7 +10979,7 @@
         <v>0.78703703703703698</v>
       </c>
     </row>
-    <row r="14" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>189</v>
       </c>
@@ -11722,7 +11722,7 @@
         <v>0.77465277777777775</v>
       </c>
     </row>
-    <row r="15" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>189</v>
       </c>
@@ -12465,7 +12465,7 @@
         <v>0.77233796296296298</v>
       </c>
     </row>
-    <row r="16" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>171</v>
       </c>
@@ -13208,7 +13208,7 @@
         <v>0.77222222222222225</v>
       </c>
     </row>
-    <row r="17" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>189</v>
       </c>
@@ -13939,7 +13939,7 @@
         <v>0.77083333333333337</v>
       </c>
     </row>
-    <row r="18" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>173</v>
       </c>
@@ -14682,7 +14682,7 @@
         <v>0.76770833333333333</v>
       </c>
     </row>
-    <row r="19" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>166</v>
       </c>
@@ -15425,7 +15425,7 @@
         <v>0.766087962962963</v>
       </c>
     </row>
-    <row r="20" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>243</v>
       </c>
@@ -16168,7 +16168,7 @@
         <v>0.76215277777777779</v>
       </c>
     </row>
-    <row r="21" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>175</v>
       </c>
@@ -16911,7 +16911,7 @@
         <v>0.75624999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>239</v>
       </c>
@@ -17654,7 +17654,7 @@
         <v>0.75104166666666672</v>
       </c>
     </row>
-    <row r="23" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>199</v>
       </c>
@@ -18385,7 +18385,7 @@
         <v>0.73715277777777777</v>
       </c>
     </row>
-    <row r="24" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>203</v>
       </c>
@@ -19128,7 +19128,7 @@
         <v>0.73333333333333328</v>
       </c>
     </row>
-    <row r="25" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>249</v>
       </c>
@@ -19871,7 +19871,7 @@
         <v>0.72187499999999993</v>
       </c>
     </row>
-    <row r="26" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>209</v>
       </c>
@@ -20614,7 +20614,7 @@
         <v>0.71493055555555551</v>
       </c>
     </row>
-    <row r="27" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>183</v>
       </c>
@@ -21357,7 +21357,7 @@
         <v>0.7138888888888888</v>
       </c>
     </row>
-    <row r="28" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>193</v>
       </c>
@@ -22088,7 +22088,7 @@
         <v>0.70844907407407409</v>
       </c>
     </row>
-    <row r="29" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>187</v>
       </c>
@@ -22831,7 +22831,7 @@
         <v>0.703125</v>
       </c>
     </row>
-    <row r="30" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>215</v>
       </c>
@@ -23574,7 +23574,7 @@
         <v>0.69097222222222232</v>
       </c>
     </row>
-    <row r="31" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>185</v>
       </c>
@@ -24317,7 +24317,7 @@
         <v>0.68032407407407414</v>
       </c>
     </row>
-    <row r="32" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>203</v>
       </c>
@@ -25060,7 +25060,7 @@
         <v>0.6791666666666667</v>
       </c>
     </row>
-    <row r="33" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>177</v>
       </c>
@@ -25803,7 +25803,7 @@
         <v>0.67604166666666665</v>
       </c>
     </row>
-    <row r="34" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>199</v>
       </c>
@@ -26534,7 +26534,7 @@
         <v>0.65196759259259263</v>
       </c>
     </row>
-    <row r="35" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>233</v>
       </c>
@@ -27277,7 +27277,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="36" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>201</v>
       </c>
@@ -28020,7 +28020,7 @@
         <v>0.64722222222222214</v>
       </c>
     </row>
-    <row r="37" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>241</v>
       </c>
@@ -28763,7 +28763,7 @@
         <v>0.64351851851851849</v>
       </c>
     </row>
-    <row r="38" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>235</v>
       </c>
@@ -29494,7 +29494,7 @@
         <v>0.62777777777777777</v>
       </c>
     </row>
-    <row r="39" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>223</v>
       </c>
@@ -30237,7 +30237,7 @@
         <v>0.6113425925925926</v>
       </c>
     </row>
-    <row r="40" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>211</v>
       </c>
@@ -30980,7 +30980,7 @@
         <v>0.60949074074074072</v>
       </c>
     </row>
-    <row r="41" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>203</v>
       </c>
@@ -31723,7 +31723,7 @@
         <v>0.59513888888888888</v>
       </c>
     </row>
-    <row r="42" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>221</v>
       </c>
@@ -32466,7 +32466,7 @@
         <v>0.59363425925925928</v>
       </c>
     </row>
-    <row r="43" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>247</v>
       </c>
@@ -33197,7 +33197,7 @@
         <v>0.56805555555555554</v>
       </c>
     </row>
-    <row r="44" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>237</v>
       </c>
@@ -33928,7 +33928,7 @@
         <v>0.55486111111111114</v>
       </c>
     </row>
-    <row r="45" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>187</v>
       </c>
@@ -34659,7 +34659,7 @@
         <v>0.54189814814814818</v>
       </c>
     </row>
-    <row r="46" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>231</v>
       </c>
@@ -35402,7 +35402,7 @@
         <v>0.53298611111111116</v>
       </c>
     </row>
-    <row r="47" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>193</v>
       </c>
@@ -36133,7 +36133,7 @@
         <v>0.53171296296296289</v>
       </c>
     </row>
-    <row r="48" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>183</v>
       </c>
@@ -36876,7 +36876,7 @@
         <v>0.51712962962962961</v>
       </c>
     </row>
-    <row r="49" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>229</v>
       </c>
@@ -37619,7 +37619,7 @@
         <v>0.48449074074074072</v>
       </c>
     </row>
-    <row r="50" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>225</v>
       </c>
@@ -38362,7 +38362,7 @@
         <v>0.46643518518518523</v>
       </c>
     </row>
-    <row r="51" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>227</v>
       </c>
@@ -39105,7 +39105,7 @@
         <v>0.46608796296296301</v>
       </c>
     </row>
-    <row r="52" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>213</v>
       </c>
@@ -39836,7 +39836,7 @@
         <v>0.39861111111111119</v>
       </c>
     </row>
-    <row r="53" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>251</v>
       </c>
@@ -40567,7 +40567,7 @@
         <v>0.32858796296296294</v>
       </c>
     </row>
-    <row r="54" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>253</v>
       </c>
@@ -41298,7 +41298,7 @@
         <v>0.30219907407407409</v>
       </c>
     </row>
-    <row r="55" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>207</v>
       </c>
@@ -42029,7 +42029,7 @@
         <v>0.20532407407407405</v>
       </c>
     </row>
-    <row r="56" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>267</v>
       </c>
@@ -42772,7 +42772,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="57" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>259</v>
       </c>
@@ -43515,7 +43515,7 @@
         <v>0.75381944444444449</v>
       </c>
     </row>
-    <row r="58" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>179</v>
       </c>
@@ -44258,7 +44258,7 @@
         <v>0.64756944444444442</v>
       </c>
     </row>
-    <row r="59" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>265</v>
       </c>
@@ -45001,7 +45001,7 @@
         <v>0.64247685185185177</v>
       </c>
     </row>
-    <row r="60" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>191</v>
       </c>
@@ -45744,7 +45744,7 @@
         <v>0.64074074074074072</v>
       </c>
     </row>
-    <row r="61" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>181</v>
       </c>
@@ -46487,7 +46487,7 @@
         <v>0.63645833333333335</v>
       </c>
     </row>
-    <row r="62" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>265</v>
       </c>
@@ -47230,7 +47230,7 @@
         <v>0.62569444444444433</v>
       </c>
     </row>
-    <row r="63" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>209</v>
       </c>
@@ -47973,7 +47973,7 @@
         <v>0.62465277777777783</v>
       </c>
     </row>
-    <row r="64" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>255</v>
       </c>
@@ -48716,7 +48716,7 @@
         <v>0.62372685185185184</v>
       </c>
     </row>
-    <row r="65" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>219</v>
       </c>
@@ -49459,7 +49459,7 @@
         <v>0.59340277777777772</v>
       </c>
     </row>
-    <row r="66" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>267</v>
       </c>
@@ -50202,7 +50202,7 @@
         <v>0.58506944444444442</v>
       </c>
     </row>
-    <row r="67" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>269</v>
       </c>
@@ -50945,7 +50945,7 @@
         <v>0.578125</v>
       </c>
     </row>
-    <row r="68" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>263</v>
       </c>
@@ -51688,7 +51688,7 @@
         <v>0.57361111111111118</v>
       </c>
     </row>
-    <row r="69" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>233</v>
       </c>
@@ -52431,7 +52431,7 @@
         <v>0.51238425925925923</v>
       </c>
     </row>
-    <row r="70" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>261</v>
       </c>
@@ -53162,7 +53162,7 @@
         <v>0.48310185185185178</v>
       </c>
     </row>
-    <row r="71" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>197</v>
       </c>
@@ -53905,7 +53905,7 @@
         <v>0.42534722222222221</v>
       </c>
     </row>
-    <row r="72" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>259</v>
       </c>
@@ -54648,7 +54648,7 @@
         <v>0.42534722222222221</v>
       </c>
     </row>
-    <row r="73" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>201</v>
       </c>
@@ -55391,7 +55391,7 @@
         <v>0.39432870370370371</v>
       </c>
     </row>
-    <row r="74" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>195</v>
       </c>
@@ -56134,7 +56134,7 @@
         <v>0.33506944444444442</v>
       </c>
     </row>
-    <row r="75" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>197</v>
       </c>
@@ -56865,7 +56865,7 @@
         <v>0.27048611111111109</v>
       </c>
     </row>
-    <row r="76" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>263</v>
       </c>
@@ -57596,7 +57596,7 @@
         <v>0.25023148148148144</v>
       </c>
     </row>
-    <row r="77" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>195</v>
       </c>
@@ -58327,7 +58327,7 @@
         <v>0.23854166666666665</v>
       </c>
     </row>
-    <row r="78" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>185</v>
       </c>
@@ -59058,7 +59058,7 @@
         <v>0.17256944444444441</v>
       </c>
     </row>
-    <row r="79" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>249</v>
       </c>
@@ -59789,7 +59789,7 @@
         <v>0.12499999999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>205</v>
       </c>
@@ -60520,7 +60520,7 @@
         <v>0.3666666666666667</v>
       </c>
     </row>
-    <row r="81" spans="1:249" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:249" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>217</v>
       </c>

</xml_diff>